<commit_message>
added vision and support for all ui funcs
</commit_message>
<xml_diff>
--- a/secrets/accounts/decrypted/accs.xlsx
+++ b/secrets/accounts/decrypted/accs.xlsx
@@ -17,12 +17,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>Account</t>
   </si>
   <si>
     <t>Adspower Browser Id</t>
+  </si>
+  <si>
+    <t>Vision Token</t>
+  </si>
+  <si>
+    <t>Vision Folder Id</t>
+  </si>
+  <si>
+    <t>Vision Profile Id</t>
   </si>
   <si>
     <t>Proxy Type</t>
@@ -634,14 +643,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="9" width="10" customWidth="1"/>
+    <col min="2" max="12" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,6 +677,15 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -690,49 +708,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -755,82 +773,82 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -853,64 +871,64 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -933,31 +951,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -980,31 +998,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1027,31 +1045,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>